<commit_message>
Added more comments and more test to template Parser
</commit_message>
<xml_diff>
--- a/testFiles/ParseTestFiles/client_profile.xlsx
+++ b/testFiles/ParseTestFiles/client_profile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>Yes</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>1978-05-20</t>
-  </si>
-  <si>
-    <t>[BUID:305939,RID:,ORP:4/5,DTS:2018-08-07 10:05:04][1] (Client) Unable to validate against database. / (Client) Impossible de valider dans la base de données.</t>
   </si>
   <si>
     <t>Consent for Future Research/Consultation</t>
@@ -166,10 +163,10 @@
 </t>
   </si>
   <si>
-    <t>FOSS/GCMS Client ID</t>
+    <t>12345678</t>
   </si>
   <si>
-    <t>12345678</t>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -595,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q2503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="J3" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>
@@ -622,7 +619,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="8" customFormat="1" ht="99.95" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -643,119 +640,119 @@
     </row>
     <row r="2" spans="1:17" hidden="1">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.6" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="126">
+    <row r="4" spans="1:17" ht="31.5">
       <c r="A4" s="5" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>

</xml_diff>